<commit_message>
Adding CyDAQ testing results and BOM with costs
</commit_message>
<xml_diff>
--- a/src/hardware/CyDAQ/BOM/CyDAQ_2_0_BOM_Master.xlsx
+++ b/src/hardware/CyDAQ/BOM/CyDAQ_2_0_BOM_Master.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20352"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20353"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\etgRepos\etg_knowledge_base\CyDAQ 2.0\Hardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\etgRepos\master_ee_224\src\hardware\CyDAQ\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D99CA06-F89F-492A-9145-F140EE008C01}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{521E8DB5-A7EE-4912-B25D-0E4AB5B10F91}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9240"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DigiKey (itemized)" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="267">
   <si>
     <t>Manufacturer Part Number</t>
   </si>
@@ -541,15 +541,6 @@
     <t>C2012X5R1V106K085AC</t>
   </si>
   <si>
-    <t>C8, C9, C12, C13</t>
-  </si>
-  <si>
-    <t>399-1169-1-ND</t>
-  </si>
-  <si>
-    <t>C0805C104M5RACTU</t>
-  </si>
-  <si>
     <t>L1</t>
   </si>
   <si>
@@ -776,12 +767,69 @@
   </si>
   <si>
     <t>D3</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>RES SMD 470 OHM 5% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>RC0805JR-07470RL</t>
+  </si>
+  <si>
+    <t>311-470ARCT-ND</t>
+  </si>
+  <si>
+    <t>Sensor Connector</t>
+  </si>
+  <si>
+    <t>70553-0001</t>
+  </si>
+  <si>
+    <t>Molex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Housings R/A HDR 2P low profile </t>
+  </si>
+  <si>
+    <t>Power Connector</t>
+  </si>
+  <si>
+    <t>Power Connector Mate</t>
+  </si>
+  <si>
+    <t>50-57-9402</t>
+  </si>
+  <si>
+    <t>2P SINGLE ROW POSITIVE LATCH</t>
+  </si>
+  <si>
+    <t>70543-0002</t>
+  </si>
+  <si>
+    <t>3P SINGLE ROW POSITIVE LATCH</t>
+  </si>
+  <si>
+    <t>VERTICAL HDR 3P single</t>
+  </si>
+  <si>
+    <t>Sensor Connector Mate</t>
+  </si>
+  <si>
+    <t>50-57-9403</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1215,7 +1263,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1258,14 +1306,16 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1293,6 +1343,7 @@
     <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Currency" xfId="42" builtinId="4"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
@@ -1618,12 +1669,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F61"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A58" sqref="A58:XFD58"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1634,9 +1685,10 @@
     <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>88</v>
       </c>
@@ -1655,68 +1707,80 @@
       <c r="F1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="E2" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="2">
+        <v>1.1599999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B3" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E3" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="2">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B4" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="E4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="2">
+        <v>2.77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>111</v>
       </c>
@@ -1735,8 +1799,11 @@
       <c r="F5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="2">
+        <v>17.170000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>89</v>
       </c>
@@ -1755,8 +1822,11 @@
       <c r="F6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>102</v>
       </c>
@@ -1775,8 +1845,11 @@
       <c r="F7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="2">
+        <v>1.92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>90</v>
       </c>
@@ -1795,8 +1868,11 @@
       <c r="F8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="2">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>101</v>
       </c>
@@ -1815,8 +1891,11 @@
       <c r="F9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="2">
+        <v>1.83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>114</v>
       </c>
@@ -1835,8 +1914,11 @@
       <c r="F10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" s="2">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>117</v>
       </c>
@@ -1855,8 +1937,11 @@
       <c r="F11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" s="2">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>124</v>
       </c>
@@ -1875,8 +1960,11 @@
       <c r="F12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" s="2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>125</v>
       </c>
@@ -1895,8 +1983,11 @@
       <c r="F13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" s="2">
+        <v>1.19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>130</v>
       </c>
@@ -1915,8 +2006,11 @@
       <c r="F14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" s="2">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>138</v>
       </c>
@@ -1935,8 +2029,11 @@
       <c r="F15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" s="2">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>139</v>
       </c>
@@ -1955,8 +2052,11 @@
       <c r="F16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" s="2">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>143</v>
       </c>
@@ -1975,8 +2075,11 @@
       <c r="F17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="2">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>147</v>
       </c>
@@ -1995,8 +2098,11 @@
       <c r="F18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" s="2">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>152</v>
       </c>
@@ -2015,8 +2121,11 @@
       <c r="F19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" s="2">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>156</v>
       </c>
@@ -2035,8 +2144,11 @@
       <c r="F20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" s="2">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>164</v>
       </c>
@@ -2055,8 +2167,11 @@
       <c r="F21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" s="2">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>165</v>
       </c>
@@ -2075,8 +2190,11 @@
       <c r="F22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22" s="2">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>166</v>
       </c>
@@ -2095,96 +2213,111 @@
       <c r="F23">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23" s="2">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>173</v>
+        <v>91</v>
       </c>
       <c r="B24" t="s">
-        <v>175</v>
+        <v>12</v>
       </c>
       <c r="C24" t="s">
-        <v>149</v>
+        <v>13</v>
       </c>
       <c r="D24" t="s">
-        <v>174</v>
+        <v>14</v>
       </c>
       <c r="E24" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F24">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="G24" s="2">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B25" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C25" t="s">
         <v>13</v>
       </c>
       <c r="D25" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E25" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F25">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="G25" s="2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>93</v>
+        <v>190</v>
       </c>
       <c r="B26" t="s">
-        <v>16</v>
+        <v>204</v>
       </c>
       <c r="C26" t="s">
-        <v>13</v>
+        <v>178</v>
       </c>
       <c r="D26" t="s">
-        <v>17</v>
+        <v>205</v>
       </c>
       <c r="E26" t="s">
-        <v>18</v>
+        <v>206</v>
       </c>
       <c r="F26">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="G26" s="2">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B27" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
       <c r="C27" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D27" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="E27" t="s">
-        <v>209</v>
+        <v>219</v>
       </c>
       <c r="F27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27" s="2">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B28" t="s">
         <v>220</v>
       </c>
       <c r="C28" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D28" t="s">
         <v>221</v>
@@ -2195,36 +2328,42 @@
       <c r="F28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28" s="2">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B29" t="s">
+        <v>224</v>
+      </c>
+      <c r="C29" t="s">
         <v>223</v>
       </c>
-      <c r="C29" t="s">
-        <v>181</v>
-      </c>
       <c r="D29" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E29" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29" s="2">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B30" t="s">
         <v>227</v>
       </c>
       <c r="C30" t="s">
-        <v>226</v>
+        <v>178</v>
       </c>
       <c r="D30" t="s">
         <v>228</v>
@@ -2235,16 +2374,19 @@
       <c r="F30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30" s="2">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B31" t="s">
         <v>230</v>
       </c>
       <c r="C31" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D31" t="s">
         <v>231</v>
@@ -2253,78 +2395,90 @@
         <v>232</v>
       </c>
       <c r="F31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="G31" s="2">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B32" t="s">
+        <v>225</v>
+      </c>
+      <c r="C32" t="s">
+        <v>223</v>
+      </c>
+      <c r="D32" t="s">
+        <v>225</v>
+      </c>
+      <c r="E32" t="s">
+        <v>226</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32" s="2">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B33" t="s">
         <v>233</v>
       </c>
-      <c r="C32" t="s">
-        <v>181</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="C33" t="s">
+        <v>178</v>
+      </c>
+      <c r="D33" t="s">
         <v>234</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E33" t="s">
         <v>235</v>
       </c>
-      <c r="F32">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B33" t="s">
-        <v>228</v>
-      </c>
-      <c r="C33" t="s">
-        <v>226</v>
-      </c>
-      <c r="D33" t="s">
-        <v>228</v>
-      </c>
-      <c r="E33" t="s">
-        <v>229</v>
-      </c>
       <c r="F33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33" s="2">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="B34" t="s">
-        <v>236</v>
+        <v>208</v>
       </c>
       <c r="C34" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D34" t="s">
-        <v>237</v>
+        <v>209</v>
       </c>
       <c r="E34" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="F34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34" s="2">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B35" t="s">
         <v>211</v>
       </c>
       <c r="C35" t="s">
-        <v>181</v>
+        <v>36</v>
       </c>
       <c r="D35" t="s">
         <v>212</v>
@@ -2335,16 +2489,19 @@
       <c r="F35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35" s="2">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B36" t="s">
         <v>214</v>
       </c>
       <c r="C36" t="s">
-        <v>36</v>
+        <v>178</v>
       </c>
       <c r="D36" t="s">
         <v>215</v>
@@ -2355,28 +2512,34 @@
       <c r="F36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G36" s="2">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>196</v>
+        <v>250</v>
       </c>
       <c r="B37" t="s">
-        <v>217</v>
+        <v>252</v>
       </c>
       <c r="C37" t="s">
-        <v>181</v>
+        <v>56</v>
       </c>
       <c r="D37" t="s">
-        <v>218</v>
+        <v>253</v>
       </c>
       <c r="E37" t="s">
-        <v>219</v>
+        <v>251</v>
       </c>
       <c r="F37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G37" s="2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>95</v>
       </c>
@@ -2395,8 +2558,11 @@
       <c r="F38">
         <v>2</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G38" s="2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>92</v>
       </c>
@@ -2415,10 +2581,13 @@
       <c r="F39">
         <v>19</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G39" s="2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B40" t="s">
         <v>23</v>
@@ -2435,8 +2604,11 @@
       <c r="F40">
         <v>20</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G40" s="2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>94</v>
       </c>
@@ -2455,8 +2627,11 @@
       <c r="F41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G41" s="2">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>103</v>
       </c>
@@ -2475,8 +2650,11 @@
       <c r="F42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G42" s="2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>104</v>
       </c>
@@ -2495,8 +2673,11 @@
       <c r="F43">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G43" s="2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>105</v>
       </c>
@@ -2515,8 +2696,11 @@
       <c r="F44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G44" s="2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>106</v>
       </c>
@@ -2535,8 +2719,11 @@
       <c r="F45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G45" s="2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>96</v>
       </c>
@@ -2555,8 +2742,11 @@
       <c r="F46">
         <v>2</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G46" s="2">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>97</v>
       </c>
@@ -2575,8 +2765,11 @@
       <c r="F47">
         <v>2</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G47" s="2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>98</v>
       </c>
@@ -2595,8 +2788,11 @@
       <c r="F48">
         <v>3</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G48" s="2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>99</v>
       </c>
@@ -2615,8 +2811,11 @@
       <c r="F49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G49" s="2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>107</v>
       </c>
@@ -2635,8 +2834,11 @@
       <c r="F50">
         <v>11</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G50" s="2">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>109</v>
       </c>
@@ -2655,8 +2857,11 @@
       <c r="F51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G51" s="2">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>110</v>
       </c>
@@ -2675,88 +2880,103 @@
       <c r="F52">
         <v>3</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G52" s="2">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B53" t="s">
+        <v>177</v>
+      </c>
+      <c r="C53" t="s">
+        <v>178</v>
+      </c>
+      <c r="D53" t="s">
+        <v>179</v>
+      </c>
+      <c r="E53" t="s">
         <v>180</v>
       </c>
-      <c r="C53" t="s">
+      <c r="F53">
+        <v>1</v>
+      </c>
+      <c r="G53" s="2">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B54" t="s">
         <v>181</v>
-      </c>
-      <c r="D53" t="s">
-        <v>182</v>
-      </c>
-      <c r="E53" t="s">
-        <v>183</v>
-      </c>
-      <c r="F53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="B54" t="s">
-        <v>184</v>
       </c>
       <c r="C54" t="s">
         <v>120</v>
       </c>
       <c r="D54" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E54" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="F54">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G54" s="2">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B55" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C55" t="s">
         <v>120</v>
       </c>
       <c r="D55" t="s">
+        <v>185</v>
+      </c>
+      <c r="E55" t="s">
+        <v>186</v>
+      </c>
+      <c r="F55">
+        <v>1</v>
+      </c>
+      <c r="G55" s="2">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B56" t="s">
+        <v>187</v>
+      </c>
+      <c r="C56" t="s">
+        <v>178</v>
+      </c>
+      <c r="D56" t="s">
         <v>188</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E56" t="s">
         <v>189</v>
       </c>
-      <c r="F55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="B56" t="s">
-        <v>190</v>
-      </c>
-      <c r="C56" t="s">
-        <v>181</v>
-      </c>
-      <c r="D56" t="s">
-        <v>191</v>
-      </c>
-      <c r="E56" t="s">
-        <v>192</v>
-      </c>
       <c r="F56">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G56" s="2">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>108</v>
       </c>
@@ -2775,28 +2995,34 @@
       <c r="F57">
         <v>2</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G57" s="2">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B58" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C58" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D58" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E58" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="F58">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G58" s="2">
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>100</v>
       </c>
@@ -2815,8 +3041,84 @@
       <c r="F59">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="G59" s="2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B61" t="s">
+        <v>255</v>
+      </c>
+      <c r="C61" t="s">
+        <v>256</v>
+      </c>
+      <c r="E61" t="s">
+        <v>257</v>
+      </c>
+      <c r="F61">
+        <v>1</v>
+      </c>
+      <c r="G61" s="2">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B62" t="s">
+        <v>260</v>
+      </c>
+      <c r="C62" t="s">
+        <v>256</v>
+      </c>
+      <c r="E62" t="s">
+        <v>261</v>
+      </c>
+      <c r="G62" s="2">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B63" t="s">
+        <v>262</v>
+      </c>
+      <c r="C63" t="s">
+        <v>256</v>
+      </c>
+      <c r="E63" t="s">
+        <v>264</v>
+      </c>
+      <c r="F63">
+        <v>3</v>
+      </c>
+      <c r="G63" s="2">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B64" t="s">
+        <v>266</v>
+      </c>
+      <c r="C64" t="s">
+        <v>256</v>
+      </c>
+      <c r="E64" t="s">
+        <v>263</v>
+      </c>
+      <c r="G64" s="2">
+        <v>0.13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated J18:20 in BOM and added filter test spreadsheet
</commit_message>
<xml_diff>
--- a/src/hardware/CyDAQ/BOM/CyDAQ_2_0_BOM_Master.xlsx
+++ b/src/hardware/CyDAQ/BOM/CyDAQ_2_0_BOM_Master.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20353"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\etgRepos\master_ee_224\src\hardware\CyDAQ\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ETG-Git-Repos\master_ee_224\src\hardware\CyDAQ\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{521E8DB5-A7EE-4912-B25D-0E4AB5B10F91}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E5B29B-A489-45E0-B523-5FC6DACDD545}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -262,18 +262,9 @@
     <t>CONN JACK STEREO 3.5MM R/A</t>
   </si>
   <si>
-    <t>SSQ-103-02-T-D-RA</t>
-  </si>
-  <si>
     <t>Samtec Inc.</t>
   </si>
   <si>
-    <t>SAM1224-03-ND</t>
-  </si>
-  <si>
-    <t>CONN RCPT 6POS 0.1 TIN PCB R/A</t>
-  </si>
-  <si>
     <t>X9258TS24IZ-2.7</t>
   </si>
   <si>
@@ -821,6 +812,15 @@
   </si>
   <si>
     <t>50-57-9403</t>
+  </si>
+  <si>
+    <t>SSW-103-01-T-D</t>
+  </si>
+  <si>
+    <t>SAM1212-03-ND</t>
+  </si>
+  <si>
+    <t>CONN RCPT 6POS 0.1 TIN PCB</t>
   </si>
 </sst>
 </file>
@@ -1673,8 +1673,8 @@
   <dimension ref="A1:G64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B74" sqref="B74"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1690,7 +1690,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1708,24 +1708,24 @@
         <v>3</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B2" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="E2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -1736,19 +1736,19 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="E3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -1759,19 +1759,19 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B4" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E4" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -1782,19 +1782,19 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" t="s">
         <v>84</v>
-      </c>
-      <c r="C5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D5" t="s">
-        <v>86</v>
-      </c>
-      <c r="E5" t="s">
-        <v>87</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -1805,7 +1805,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -1828,7 +1828,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
         <v>52</v>
@@ -1851,7 +1851,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -1874,7 +1874,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B9" t="s">
         <v>49</v>
@@ -1897,19 +1897,19 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B10" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C10" t="s">
         <v>13</v>
       </c>
       <c r="D10" t="s">
+        <v>109</v>
+      </c>
+      <c r="E10" t="s">
         <v>112</v>
-      </c>
-      <c r="E10" t="s">
-        <v>115</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -1920,19 +1920,19 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C11" t="s">
         <v>117</v>
       </c>
-      <c r="B11" t="s">
+      <c r="D11" t="s">
         <v>116</v>
       </c>
-      <c r="C11" t="s">
-        <v>120</v>
-      </c>
-      <c r="D11" t="s">
-        <v>119</v>
-      </c>
       <c r="E11" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F11">
         <v>2</v>
@@ -1943,19 +1943,19 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B12" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D12" t="s">
+        <v>118</v>
+      </c>
+      <c r="E12" t="s">
         <v>120</v>
-      </c>
-      <c r="D12" t="s">
-        <v>121</v>
-      </c>
-      <c r="E12" t="s">
-        <v>123</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -1966,19 +1966,19 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B13" t="s">
+        <v>123</v>
+      </c>
+      <c r="C13" t="s">
+        <v>124</v>
+      </c>
+      <c r="D13" t="s">
+        <v>126</v>
+      </c>
+      <c r="E13" t="s">
         <v>125</v>
-      </c>
-      <c r="B13" t="s">
-        <v>126</v>
-      </c>
-      <c r="C13" t="s">
-        <v>127</v>
-      </c>
-      <c r="D13" t="s">
-        <v>129</v>
-      </c>
-      <c r="E13" t="s">
-        <v>128</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -1989,19 +1989,19 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B14" t="s">
+        <v>131</v>
+      </c>
+      <c r="C14" t="s">
+        <v>129</v>
+      </c>
+      <c r="D14" t="s">
+        <v>128</v>
+      </c>
+      <c r="E14" t="s">
         <v>130</v>
-      </c>
-      <c r="B14" t="s">
-        <v>134</v>
-      </c>
-      <c r="C14" t="s">
-        <v>132</v>
-      </c>
-      <c r="D14" t="s">
-        <v>131</v>
-      </c>
-      <c r="E14" t="s">
-        <v>133</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -2012,19 +2012,19 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B15" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C15" t="s">
+        <v>129</v>
+      </c>
+      <c r="D15" t="s">
         <v>132</v>
       </c>
-      <c r="D15" t="s">
-        <v>135</v>
-      </c>
       <c r="E15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -2035,19 +2035,19 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B16" t="s">
         <v>139</v>
       </c>
-      <c r="B16" t="s">
-        <v>142</v>
-      </c>
       <c r="C16" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D16" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E16" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -2058,19 +2058,19 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B17" t="s">
+        <v>141</v>
+      </c>
+      <c r="C17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D17" t="s">
+        <v>142</v>
+      </c>
+      <c r="E17" t="s">
         <v>143</v>
-      </c>
-      <c r="B17" t="s">
-        <v>144</v>
-      </c>
-      <c r="C17" t="s">
-        <v>132</v>
-      </c>
-      <c r="D17" t="s">
-        <v>145</v>
-      </c>
-      <c r="E17" t="s">
-        <v>146</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -2081,19 +2081,19 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B18" t="s">
+        <v>145</v>
+      </c>
+      <c r="C18" t="s">
+        <v>146</v>
+      </c>
+      <c r="D18" t="s">
         <v>147</v>
       </c>
-      <c r="B18" t="s">
+      <c r="E18" t="s">
         <v>148</v>
-      </c>
-      <c r="C18" t="s">
-        <v>149</v>
-      </c>
-      <c r="D18" t="s">
-        <v>150</v>
-      </c>
-      <c r="E18" t="s">
-        <v>151</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -2104,19 +2104,19 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B19" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C19" t="s">
         <v>13</v>
       </c>
       <c r="D19" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E19" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -2127,19 +2127,19 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B20" t="s">
+        <v>155</v>
+      </c>
+      <c r="C20" t="s">
         <v>156</v>
       </c>
-      <c r="B20" t="s">
-        <v>158</v>
-      </c>
-      <c r="C20" t="s">
-        <v>159</v>
-      </c>
       <c r="D20" t="s">
+        <v>154</v>
+      </c>
+      <c r="E20" t="s">
         <v>157</v>
-      </c>
-      <c r="E20" t="s">
-        <v>160</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -2150,19 +2150,19 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B21" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C21" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D21" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E21" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F21">
         <v>1</v>
@@ -2173,19 +2173,19 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B22" t="s">
+        <v>164</v>
+      </c>
+      <c r="C22" t="s">
+        <v>124</v>
+      </c>
+      <c r="D22" t="s">
         <v>165</v>
       </c>
-      <c r="B22" t="s">
-        <v>167</v>
-      </c>
-      <c r="C22" t="s">
-        <v>127</v>
-      </c>
-      <c r="D22" t="s">
-        <v>168</v>
-      </c>
       <c r="E22" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F22">
         <v>1</v>
@@ -2196,19 +2196,19 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B23" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C23" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D23" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E23" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F23">
         <v>2</v>
@@ -2219,7 +2219,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B24" t="s">
         <v>12</v>
@@ -2242,7 +2242,7 @@
     </row>
     <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B25" t="s">
         <v>16</v>
@@ -2265,19 +2265,19 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B26" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C26" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D26" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E26" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F26">
         <v>1</v>
@@ -2288,19 +2288,19 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B27" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C27" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D27" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E27" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="F27">
         <v>1</v>
@@ -2311,19 +2311,19 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B28" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C28" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D28" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E28" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F28">
         <v>1</v>
@@ -2334,19 +2334,19 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B29" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C29" t="s">
+        <v>220</v>
+      </c>
+      <c r="D29" t="s">
+        <v>222</v>
+      </c>
+      <c r="E29" t="s">
         <v>223</v>
-      </c>
-      <c r="D29" t="s">
-        <v>225</v>
-      </c>
-      <c r="E29" t="s">
-        <v>226</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -2357,19 +2357,19 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B30" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C30" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D30" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E30" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="F30">
         <v>1</v>
@@ -2380,19 +2380,19 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B31" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C31" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D31" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E31" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="F31">
         <v>2</v>
@@ -2403,19 +2403,19 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B32" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C32" t="s">
+        <v>220</v>
+      </c>
+      <c r="D32" t="s">
+        <v>222</v>
+      </c>
+      <c r="E32" t="s">
         <v>223</v>
-      </c>
-      <c r="D32" t="s">
-        <v>225</v>
-      </c>
-      <c r="E32" t="s">
-        <v>226</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -2426,19 +2426,19 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B33" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C33" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D33" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="E33" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="F33">
         <v>1</v>
@@ -2449,19 +2449,19 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B34" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C34" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D34" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E34" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="F34">
         <v>1</v>
@@ -2472,19 +2472,19 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B35" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C35" t="s">
         <v>36</v>
       </c>
       <c r="D35" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E35" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="F35">
         <v>1</v>
@@ -2495,19 +2495,19 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B36" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C36" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D36" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E36" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="F36">
         <v>1</v>
@@ -2518,19 +2518,19 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B37" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C37" t="s">
         <v>56</v>
       </c>
       <c r="D37" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="E37" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F37">
         <v>1</v>
@@ -2541,7 +2541,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B38" t="s">
         <v>29</v>
@@ -2564,7 +2564,7 @@
     </row>
     <row r="39" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B39" t="s">
         <v>19</v>
@@ -2587,7 +2587,7 @@
     </row>
     <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B40" t="s">
         <v>23</v>
@@ -2610,7 +2610,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B41" t="s">
         <v>26</v>
@@ -2633,7 +2633,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B42" t="s">
         <v>55</v>
@@ -2656,7 +2656,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B43" t="s">
         <v>59</v>
@@ -2679,7 +2679,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B44" t="s">
         <v>62</v>
@@ -2702,7 +2702,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B45" t="s">
         <v>65</v>
@@ -2725,7 +2725,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B46" t="s">
         <v>32</v>
@@ -2748,7 +2748,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B47" t="s">
         <v>35</v>
@@ -2771,7 +2771,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B48" t="s">
         <v>39</v>
@@ -2794,7 +2794,7 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B49" t="s">
         <v>42</v>
@@ -2817,7 +2817,7 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B50" t="s">
         <v>68</v>
@@ -2840,7 +2840,7 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B51" t="s">
         <v>76</v>
@@ -2863,42 +2863,42 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B52" t="s">
+        <v>264</v>
+      </c>
+      <c r="C52" t="s">
         <v>80</v>
       </c>
-      <c r="C52" t="s">
-        <v>81</v>
-      </c>
       <c r="D52" t="s">
-        <v>82</v>
+        <v>265</v>
       </c>
       <c r="E52" t="s">
-        <v>83</v>
+        <v>266</v>
       </c>
       <c r="F52">
         <v>3</v>
       </c>
       <c r="G52" s="2">
-        <v>0.52</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B53" t="s">
+        <v>174</v>
+      </c>
+      <c r="C53" t="s">
+        <v>175</v>
+      </c>
+      <c r="D53" t="s">
+        <v>176</v>
+      </c>
+      <c r="E53" t="s">
         <v>177</v>
-      </c>
-      <c r="C53" t="s">
-        <v>178</v>
-      </c>
-      <c r="D53" t="s">
-        <v>179</v>
-      </c>
-      <c r="E53" t="s">
-        <v>180</v>
       </c>
       <c r="F53">
         <v>1</v>
@@ -2909,19 +2909,19 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B54" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C54" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D54" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E54" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F54">
         <v>1</v>
@@ -2932,19 +2932,19 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B55" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C55" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D55" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E55" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="F55">
         <v>1</v>
@@ -2955,19 +2955,19 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B56" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C56" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D56" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E56" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F56">
         <v>1</v>
@@ -2978,7 +2978,7 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B57" t="s">
         <v>72</v>
@@ -3001,19 +3001,19 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B58" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C58" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D58" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E58" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F58">
         <v>1</v>
@@ -3024,7 +3024,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B59" t="s">
         <v>45</v>
@@ -3047,16 +3047,16 @@
     </row>
     <row r="61" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B61" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C61" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E61" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="F61">
         <v>1</v>
@@ -3067,16 +3067,16 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B62" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C62" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E62" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="G62" s="2">
         <v>0.16</v>
@@ -3084,16 +3084,16 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B63" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C63" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E63" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="F63">
         <v>3</v>
@@ -3104,16 +3104,16 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B64" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C64" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E64" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="G64" s="2">
         <v>0.13</v>

</xml_diff>